<commit_message>
Added The automation stracture , login , register , forget
</commit_message>
<xml_diff>
--- a/manual-testing/Test Cases _ ParaBank.xlsx
+++ b/manual-testing/Test Cases _ ParaBank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebra\OneDrive\Desktop\para-bank-restful-booker-testing\manual-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E57D9BB-ECD9-48DC-8883-2C8806AAD7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7406FD8-1200-4011-97DB-6315EA2EB973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{37256061-E2C9-42E7-ACD7-E41E548C7EED}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{37256061-E2C9-42E7-ACD7-E41E548C7EED}"/>
   </bookViews>
   <sheets>
     <sheet name="Login page" sheetId="6" r:id="rId1"/>
@@ -4318,8 +4318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9709CC-42A4-487A-B23F-9A8D5A7B910F}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="61" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>